<commit_message>
mandelbrot set with three execution models
</commit_message>
<xml_diff>
--- a/MS/MS_data.xlsx
+++ b/MS/MS_data.xlsx
@@ -375,10 +375,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>simd2_manually</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>ulo1_2 manually</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -387,10 +383,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>simd2_v2_manually</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>ulo2_1 manually</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -427,10 +419,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>use channel to transfer framebuffer[640+800] (output)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>55,308 / 427,200 ( 13 % )</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -495,6 +483,18 @@
   </si>
   <si>
     <t>4-1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>simd2m</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>simd2m_v2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>use channel to transfer framebuffer[640*800] (output)</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -950,8 +950,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K84"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="B31" sqref="B31"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1401,10 +1401,10 @@
     </row>
     <row r="17" spans="1:11" s="8" customFormat="1" ht="31.5" x14ac:dyDescent="0.15">
       <c r="A17" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="B17" s="1" t="s">
         <v>79</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>80</v>
       </c>
       <c r="C17" s="1">
         <v>87336</v>
@@ -1413,7 +1413,7 @@
         <v>109259</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="F17" s="1" t="s">
         <v>25</v>
@@ -1437,10 +1437,10 @@
     </row>
     <row r="18" spans="1:11" s="8" customFormat="1" ht="31.5" x14ac:dyDescent="0.15">
       <c r="A18" s="1" t="s">
-        <v>82</v>
+        <v>108</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C18" s="1">
         <v>89186</v>
@@ -1449,7 +1449,7 @@
         <v>111807</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="F18" s="1" t="s">
         <v>28</v>
@@ -1473,7 +1473,7 @@
     </row>
     <row r="19" spans="1:11" s="8" customFormat="1" ht="31.5" x14ac:dyDescent="0.15">
       <c r="A19" s="1" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B19" s="1"/>
       <c r="C19" s="1">
@@ -1507,7 +1507,7 @@
     </row>
     <row r="20" spans="1:11" s="8" customFormat="1" ht="31.5" x14ac:dyDescent="0.15">
       <c r="A20" s="1" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B20" s="1"/>
       <c r="C20" s="1">
@@ -1517,7 +1517,7 @@
         <v>112528</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="F20" s="1" t="s">
         <v>22</v>
@@ -1580,7 +1580,7 @@
     </row>
     <row r="24" spans="1:11" s="3" customFormat="1" ht="10.5" x14ac:dyDescent="0.15">
       <c r="A24" s="3" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B24" s="3">
         <v>7</v>
@@ -1591,10 +1591,10 @@
     </row>
     <row r="25" spans="1:11" s="1" customFormat="1" ht="31.5" x14ac:dyDescent="0.15">
       <c r="A25" s="5" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C25" s="6" t="s">
         <v>0</v>
@@ -1626,10 +1626,10 @@
     </row>
     <row r="26" spans="1:11" s="8" customFormat="1" ht="31.5" x14ac:dyDescent="0.15">
       <c r="A26" s="10" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>92</v>
+        <v>109</v>
       </c>
       <c r="C26" s="1">
         <v>74771</v>
@@ -1638,16 +1638,16 @@
         <v>91355</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="G26" s="1" t="s">
         <v>18</v>
       </c>
       <c r="H26" s="1" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="I26" s="14">
         <v>263.88888888899999</v>
@@ -1662,10 +1662,10 @@
     </row>
     <row r="27" spans="1:11" s="8" customFormat="1" ht="31.5" x14ac:dyDescent="0.15">
       <c r="A27" s="10" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="B27" s="8" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="C27" s="1">
         <v>145274</v>
@@ -1674,7 +1674,7 @@
         <v>176769</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="F27" s="7" t="s">
         <v>32</v>
@@ -1701,7 +1701,7 @@
         <v>35</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="C28" s="1">
         <v>75077</v>
@@ -1710,10 +1710,10 @@
         <v>91427</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="F28" s="7" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="G28" s="1" t="s">
         <v>23</v>
@@ -1734,10 +1734,10 @@
     </row>
     <row r="29" spans="1:11" s="8" customFormat="1" ht="31.5" x14ac:dyDescent="0.15">
       <c r="A29" s="10" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="B29" s="8" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="C29" s="1">
         <v>137655</v>
@@ -1746,7 +1746,7 @@
         <v>161182</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="F29" s="1" t="s">
         <v>32</v>
@@ -1770,10 +1770,10 @@
     </row>
     <row r="30" spans="1:11" s="20" customFormat="1" ht="31.5" x14ac:dyDescent="0.15">
       <c r="A30" s="11" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="B30" s="20" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="C30" s="3">
         <v>390961</v>
@@ -1782,7 +1782,7 @@
         <v>457335</v>
       </c>
       <c r="E30" s="3" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="F30" s="3" t="s">
         <v>24</v>
@@ -1815,13 +1815,13 @@
         <v>93862</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="F31" s="1" t="s">
         <v>17</v>
       </c>
       <c r="G31" s="1" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="H31" s="1" t="s">
         <v>30</v>
@@ -1848,7 +1848,7 @@
         <v>167165</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="F32" s="7" t="s">
         <v>32</v>

</xml_diff>